<commit_message>
Atualizado IE-CEP e IP-CLF_1_2.XLSX
</commit_message>
<xml_diff>
--- a/outputs/autoaprop.xlsx/autoapropxlsx/IE-CEP.XLSX
+++ b/outputs/autoaprop.xlsx/autoapropxlsx/IE-CEP.XLSX
@@ -198,9 +198,6 @@
     <t>DYANA LUIZA</t>
   </si>
   <si>
-    <t>JULIANA OLIVEIRA</t>
-  </si>
-  <si>
     <t>GREGORY VIANNA CEZAR</t>
   </si>
   <si>
@@ -216,6 +213,18 @@
     <t>FELIPE DE OLIVEIRA MARCIANO</t>
   </si>
   <si>
+    <t>ANGELO ESTEVES DA SILVA</t>
+  </si>
+  <si>
+    <t>PRISCILA SILVA DE SOUZA</t>
+  </si>
+  <si>
+    <t>PEDRO CRUZ DA SILVA</t>
+  </si>
+  <si>
+    <t>TAYNÁ ARAUJO PINTO</t>
+  </si>
+  <si>
     <t> </t>
   </si>
   <si>
@@ -231,15 +240,6 @@
     <t> </t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
     <t>1698</t>
   </si>
   <si>
@@ -288,9 +288,6 @@
     <t>3514</t>
   </si>
   <si>
-    <t>3519</t>
-  </si>
-  <si>
     <t>3592</t>
   </si>
   <si>
@@ -306,13 +303,16 @@
     <t>3719</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
+    <t>4139</t>
+  </si>
+  <si>
+    <t>4159</t>
+  </si>
+  <si>
+    <t>4161</t>
+  </si>
+  <si>
+    <t>4173</t>
   </si>
   <si>
     <t> </t>

</xml_diff>